<commit_message>
Last commit TP Blockchain
</commit_message>
<xml_diff>
--- a/canvas/Canvas TP 1.xlsx
+++ b/canvas/Canvas TP 1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -702,7 +702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>